<commit_message>
Data migration for currencies.
</commit_message>
<xml_diff>
--- a/xconverter/currencies.xlsx
+++ b/xconverter/currencies.xlsx
@@ -1674,15 +1674,6 @@
     <t>ZWD</t>
   </si>
   <si>
-    <t>PAYS</t>
-  </si>
-  <si>
-    <t>DEVISE</t>
-  </si>
-  <si>
-    <t>ISO</t>
-  </si>
-  <si>
     <t>Livre turque</t>
   </si>
   <si>
@@ -1702,6 +1693,15 @@
   </si>
   <si>
     <t>ZMK</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>iso</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
 </sst>
 </file>
@@ -2114,7 +2114,7 @@
   <dimension ref="A1:C237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -2127,13 +2127,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21">
@@ -2584,7 +2584,7 @@
         <v>112</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="21">
@@ -2614,7 +2614,7 @@
         <v>117</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>118</v>
@@ -3761,7 +3761,7 @@
         <v>358</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21">
@@ -4099,7 +4099,7 @@
         <v>421</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>422</v>
@@ -4605,7 +4605,7 @@
         <v>524</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>525</v>
@@ -4715,10 +4715,10 @@
         <v>547</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="21">

</xml_diff>